<commit_message>
Added new temperature sensors into the database
</commit_message>
<xml_diff>
--- a/UHA.xlsx
+++ b/UHA.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="304">
   <si>
     <t>dec</t>
   </si>
@@ -911,6 +911,24 @@
   </si>
   <si>
     <t>VAR_METEO_WIND_ENERGY</t>
+  </si>
+  <si>
+    <t>VAR_TEMP_RECU_FC</t>
+  </si>
+  <si>
+    <t>VAR_TEMP_RECU_FH</t>
+  </si>
+  <si>
+    <t>VAR_TEMP_RECU_WH</t>
+  </si>
+  <si>
+    <t>VAR_TEMP_RECU_WC</t>
+  </si>
+  <si>
+    <t>T305</t>
+  </si>
+  <si>
+    <t>T309</t>
   </si>
 </sst>
 </file>
@@ -1429,8 +1447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:P259"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E126" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N165" sqref="N165:N168"/>
+    <sheetView tabSelected="1" topLeftCell="A114" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I150" sqref="I150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1440,7 +1458,7 @@
     <col min="8" max="8" width="45.5703125" customWidth="1"/>
     <col min="9" max="9" width="49.42578125" customWidth="1"/>
     <col min="11" max="11" width="3.5703125" customWidth="1"/>
-    <col min="12" max="12" width="16.42578125" customWidth="1"/>
+    <col min="12" max="12" width="35.85546875" customWidth="1"/>
     <col min="13" max="13" width="34.140625" customWidth="1"/>
     <col min="14" max="14" width="86" customWidth="1"/>
     <col min="15" max="15" width="5" customWidth="1"/>
@@ -3528,7 +3546,7 @@
         <v>public const byte VAR_EL_HEATER_STATUS = 80;</v>
       </c>
       <c r="L84" t="str">
-        <f t="shared" ref="L84:L131" si="12">CONCATENATE("UpdateScanList(",E84, ", 3000);")</f>
+        <f t="shared" ref="L84:L132" si="12">CONCATENATE("UpdateScanList(",E84, ", 3000);")</f>
         <v>UpdateScanList(VAR_EL_HEATER_STATUS, 3000);</v>
       </c>
       <c r="N84" t="str">
@@ -3536,7 +3554,7 @@
         <v>COM_AddStreamedVariable(VAR_EL_HEATER_STATUS, 1000);</v>
       </c>
       <c r="P84" t="str">
-        <f t="shared" ref="P84:P131" si="13">CONCATENATE("cJSON_AddItemToObject(Uha, ","""",E84,"""",", cJSON_CreateNumber(mVars[",C84,"]));")</f>
+        <f t="shared" ref="P84:P132" si="13">CONCATENATE("cJSON_AddItemToObject(Uha, ","""",E84,"""",", cJSON_CreateNumber(mVars[",C84,"]));")</f>
         <v>cJSON_AddItemToObject(Uha, "VAR_EL_HEATER_STATUS", cJSON_CreateNumber(mVars[80]));</v>
       </c>
     </row>
@@ -4656,11 +4674,11 @@
         <v>154</v>
       </c>
       <c r="H117" t="str">
-        <f t="shared" ref="H117:H131" si="17">CONCATENATE("#define  ",E117,"  ",C117)</f>
+        <f t="shared" ref="H117:H132" si="17">CONCATENATE("#define  ",E117,"  ",C117)</f>
         <v>#define  VAR_TEMP_BOILER_EXHAUST  113</v>
       </c>
       <c r="I117" t="str">
-        <f t="shared" ref="I117:I131" si="18">CONCATENATE("public const byte ",E117," = ",C117,";")</f>
+        <f t="shared" ref="I117:I132" si="18">CONCATENATE("public const byte ",E117," = ",C117,";")</f>
         <v>public const byte VAR_TEMP_BOILER_EXHAUST = 113;</v>
       </c>
       <c r="K117" t="str">
@@ -5135,7 +5153,7 @@
         <v>UpdateScanList(VAR_TEMP_OFFICE, 3000);</v>
       </c>
       <c r="N129" t="str">
-        <f t="shared" ref="N129:N169" si="19">CONCATENATE("COM_AddStreamedVariable(",E129, ", 1000);")</f>
+        <f t="shared" ref="N129:N168" si="19">CONCATENATE("COM_AddStreamedVariable(",E129, ", 1000);")</f>
         <v>COM_AddStreamedVariable(VAR_TEMP_OFFICE, 1000);</v>
       </c>
       <c r="P129" t="str">
@@ -5238,6 +5256,29 @@
         <f t="shared" si="10"/>
         <v>80</v>
       </c>
+      <c r="E132" t="s">
+        <v>298</v>
+      </c>
+      <c r="H132" t="str">
+        <f t="shared" si="17"/>
+        <v>#define  VAR_TEMP_RECU_FC  128</v>
+      </c>
+      <c r="I132" t="str">
+        <f t="shared" si="18"/>
+        <v>public const byte VAR_TEMP_RECU_FC = 128;</v>
+      </c>
+      <c r="L132" t="str">
+        <f t="shared" si="12"/>
+        <v>UpdateScanList(VAR_TEMP_RECU_FC, 3000);</v>
+      </c>
+      <c r="N132" t="str">
+        <f t="shared" si="19"/>
+        <v>COM_AddStreamedVariable(VAR_TEMP_RECU_FC, 1000);</v>
+      </c>
+      <c r="P132" t="str">
+        <f t="shared" si="13"/>
+        <v>cJSON_AddItemToObject(Uha, "VAR_TEMP_RECU_FC", cJSON_CreateNumber(mVars[128]));</v>
+      </c>
     </row>
     <row r="133" spans="2:16">
       <c r="B133" s="15"/>
@@ -5248,6 +5289,29 @@
         <f t="shared" ref="D133:D196" si="20">DEC2HEX(C133,2)</f>
         <v>81</v>
       </c>
+      <c r="E133" t="s">
+        <v>299</v>
+      </c>
+      <c r="H133" t="str">
+        <f t="shared" ref="H133:H137" si="21">CONCATENATE("#define  ",E133,"  ",C133)</f>
+        <v>#define  VAR_TEMP_RECU_FH  129</v>
+      </c>
+      <c r="I133" t="str">
+        <f t="shared" ref="I133:I137" si="22">CONCATENATE("public const byte ",E133," = ",C133,";")</f>
+        <v>public const byte VAR_TEMP_RECU_FH = 129;</v>
+      </c>
+      <c r="L133" t="str">
+        <f t="shared" ref="L133:L137" si="23">CONCATENATE("UpdateScanList(",E133, ", 3000);")</f>
+        <v>UpdateScanList(VAR_TEMP_RECU_FH, 3000);</v>
+      </c>
+      <c r="N133" t="str">
+        <f t="shared" ref="N133:N137" si="24">CONCATENATE("COM_AddStreamedVariable(",E133, ", 1000);")</f>
+        <v>COM_AddStreamedVariable(VAR_TEMP_RECU_FH, 1000);</v>
+      </c>
+      <c r="P133" t="str">
+        <f t="shared" ref="P133:P137" si="25">CONCATENATE("cJSON_AddItemToObject(Uha, ","""",E133,"""",", cJSON_CreateNumber(mVars[",C133,"]));")</f>
+        <v>cJSON_AddItemToObject(Uha, "VAR_TEMP_RECU_FH", cJSON_CreateNumber(mVars[129]));</v>
+      </c>
     </row>
     <row r="134" spans="2:16">
       <c r="B134" s="15"/>
@@ -5258,6 +5322,32 @@
         <f t="shared" si="20"/>
         <v>82</v>
       </c>
+      <c r="E134" t="s">
+        <v>300</v>
+      </c>
+      <c r="F134" t="s">
+        <v>303</v>
+      </c>
+      <c r="H134" t="str">
+        <f t="shared" si="21"/>
+        <v>#define  VAR_TEMP_RECU_WH  130</v>
+      </c>
+      <c r="I134" t="str">
+        <f t="shared" si="22"/>
+        <v>public const byte VAR_TEMP_RECU_WH = 130;</v>
+      </c>
+      <c r="L134" t="str">
+        <f t="shared" si="23"/>
+        <v>UpdateScanList(VAR_TEMP_RECU_WH, 3000);</v>
+      </c>
+      <c r="N134" t="str">
+        <f t="shared" si="24"/>
+        <v>COM_AddStreamedVariable(VAR_TEMP_RECU_WH, 1000);</v>
+      </c>
+      <c r="P134" t="str">
+        <f t="shared" si="25"/>
+        <v>cJSON_AddItemToObject(Uha, "VAR_TEMP_RECU_WH", cJSON_CreateNumber(mVars[130]));</v>
+      </c>
     </row>
     <row r="135" spans="2:16">
       <c r="B135" s="15"/>
@@ -5268,6 +5358,32 @@
         <f t="shared" si="20"/>
         <v>83</v>
       </c>
+      <c r="E135" t="s">
+        <v>301</v>
+      </c>
+      <c r="F135" t="s">
+        <v>302</v>
+      </c>
+      <c r="H135" t="str">
+        <f t="shared" si="21"/>
+        <v>#define  VAR_TEMP_RECU_WC  131</v>
+      </c>
+      <c r="I135" t="str">
+        <f t="shared" si="22"/>
+        <v>public const byte VAR_TEMP_RECU_WC = 131;</v>
+      </c>
+      <c r="L135" t="str">
+        <f t="shared" si="23"/>
+        <v>UpdateScanList(VAR_TEMP_RECU_WC, 3000);</v>
+      </c>
+      <c r="N135" t="str">
+        <f t="shared" si="24"/>
+        <v>COM_AddStreamedVariable(VAR_TEMP_RECU_WC, 1000);</v>
+      </c>
+      <c r="P135" t="str">
+        <f t="shared" si="25"/>
+        <v>cJSON_AddItemToObject(Uha, "VAR_TEMP_RECU_WC", cJSON_CreateNumber(mVars[131]));</v>
+      </c>
     </row>
     <row r="136" spans="2:16">
       <c r="B136" s="15"/>
@@ -5573,19 +5689,19 @@
         <v>294</v>
       </c>
       <c r="H165" t="str">
-        <f t="shared" ref="H165:H183" si="21">CONCATENATE("#define  ",E165,"  ",C165)</f>
+        <f t="shared" ref="H165:H168" si="26">CONCATENATE("#define  ",E165,"  ",C165)</f>
         <v>#define  VAR_METEO_WIND_BURST  161</v>
       </c>
       <c r="I165" t="str">
-        <f t="shared" ref="I165:I183" si="22">CONCATENATE("public const byte ",E165," = ",C165,";")</f>
+        <f t="shared" ref="I165:I168" si="27">CONCATENATE("public const byte ",E165," = ",C165,";")</f>
         <v>public const byte VAR_METEO_WIND_BURST = 161;</v>
       </c>
       <c r="L165" t="str">
-        <f t="shared" ref="L165:L183" si="23">CONCATENATE("UpdateScanList(",E165, ", 3000);")</f>
+        <f t="shared" ref="L165:L168" si="28">CONCATENATE("UpdateScanList(",E165, ", 3000);")</f>
         <v>UpdateScanList(VAR_METEO_WIND_BURST, 3000);</v>
       </c>
       <c r="M165" t="str">
-        <f t="shared" ref="M165:M183" si="24">CONCATENATE("VAR_SetVariable(",E165,", Cells[",J165,"].Voltage_mV", ", validflag);")</f>
+        <f t="shared" ref="M165:M168" si="29">CONCATENATE("VAR_SetVariable(",E165,", Cells[",J165,"].Voltage_mV", ", validflag);")</f>
         <v>VAR_SetVariable(VAR_METEO_WIND_BURST, Cells[].Voltage_mV, validflag);</v>
       </c>
       <c r="N165" t="str">
@@ -5593,7 +5709,7 @@
         <v>COM_AddStreamedVariable(VAR_METEO_WIND_BURST, 1000);</v>
       </c>
       <c r="P165" t="str">
-        <f t="shared" ref="P165:P183" si="25">CONCATENATE("cJSON_AddItemToObject(Uha, ","""",E165,"""",", cJSON_CreateNumber(mVars[",C165,"]));")</f>
+        <f t="shared" ref="P165:P168" si="30">CONCATENATE("cJSON_AddItemToObject(Uha, ","""",E165,"""",", cJSON_CreateNumber(mVars[",C165,"]));")</f>
         <v>cJSON_AddItemToObject(Uha, "VAR_METEO_WIND_BURST", cJSON_CreateNumber(mVars[161]));</v>
       </c>
     </row>
@@ -5609,19 +5725,19 @@
         <v>295</v>
       </c>
       <c r="H166" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>#define  VAR_METEO_WIND_AVG  162</v>
       </c>
       <c r="I166" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>public const byte VAR_METEO_WIND_AVG = 162;</v>
       </c>
       <c r="L166" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>UpdateScanList(VAR_METEO_WIND_AVG, 3000);</v>
       </c>
       <c r="M166" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>VAR_SetVariable(VAR_METEO_WIND_AVG, Cells[].Voltage_mV, validflag);</v>
       </c>
       <c r="N166" t="str">
@@ -5629,7 +5745,7 @@
         <v>COM_AddStreamedVariable(VAR_METEO_WIND_AVG, 1000);</v>
       </c>
       <c r="P166" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_METEO_WIND_AVG", cJSON_CreateNumber(mVars[162]));</v>
       </c>
     </row>
@@ -5645,19 +5761,19 @@
         <v>296</v>
       </c>
       <c r="H167" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>#define  VAR_METEO_WIND_POW  163</v>
       </c>
       <c r="I167" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>public const byte VAR_METEO_WIND_POW = 163;</v>
       </c>
       <c r="L167" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>UpdateScanList(VAR_METEO_WIND_POW, 3000);</v>
       </c>
       <c r="M167" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>VAR_SetVariable(VAR_METEO_WIND_POW, Cells[].Voltage_mV, validflag);</v>
       </c>
       <c r="N167" t="str">
@@ -5665,7 +5781,7 @@
         <v>COM_AddStreamedVariable(VAR_METEO_WIND_POW, 1000);</v>
       </c>
       <c r="P167" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_METEO_WIND_POW", cJSON_CreateNumber(mVars[163]));</v>
       </c>
     </row>
@@ -5681,19 +5797,19 @@
         <v>297</v>
       </c>
       <c r="H168" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>#define  VAR_METEO_WIND_ENERGY  164</v>
       </c>
       <c r="I168" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>public const byte VAR_METEO_WIND_ENERGY = 164;</v>
       </c>
       <c r="L168" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>UpdateScanList(VAR_METEO_WIND_ENERGY, 3000);</v>
       </c>
       <c r="M168" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>VAR_SetVariable(VAR_METEO_WIND_ENERGY, Cells[].Voltage_mV, validflag);</v>
       </c>
       <c r="N168" t="str">
@@ -5701,7 +5817,7 @@
         <v>COM_AddStreamedVariable(VAR_METEO_WIND_ENERGY, 1000);</v>
       </c>
       <c r="P168" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_METEO_WIND_ENERGY", cJSON_CreateNumber(mVars[164]));</v>
       </c>
     </row>
@@ -5852,18 +5968,18 @@
         <v>189</v>
       </c>
       <c r="H184" t="str">
-        <f t="shared" ref="H184:H195" si="26">CONCATENATE("#define  ",E184,"  ",C184)</f>
+        <f t="shared" ref="H184:H195" si="31">CONCATENATE("#define  ",E184,"  ",C184)</f>
         <v>#define  VAR_BMS1_CELL1_MV  180</v>
       </c>
       <c r="I184" t="str">
-        <f t="shared" ref="I184:I195" si="27">CONCATENATE("public const byte ",E184," = ",C184,";")</f>
+        <f t="shared" ref="I184:I195" si="32">CONCATENATE("public const byte ",E184," = ",C184,";")</f>
         <v>public const byte VAR_BMS1_CELL1_MV = 180;</v>
       </c>
       <c r="J184">
         <v>0</v>
       </c>
       <c r="L184" t="str">
-        <f t="shared" ref="L184:L206" si="28">CONCATENATE("UpdateScanList(",E184, ", 3000);")</f>
+        <f t="shared" ref="L184:L206" si="33">CONCATENATE("UpdateScanList(",E184, ", 3000);")</f>
         <v>UpdateScanList(VAR_BMS1_CELL1_MV, 3000);</v>
       </c>
       <c r="M184" t="str">
@@ -5871,7 +5987,7 @@
         <v>VAR_SetVariable(VAR_BMS1_CELL1_MV, Cells[0].Voltage_mV, validflag);</v>
       </c>
       <c r="P184" t="str">
-        <f t="shared" ref="P184:P206" si="29">CONCATENATE("cJSON_AddItemToObject(Uha, ","""",E184,"""",", cJSON_CreateNumber(mVars[",C184,"]));")</f>
+        <f t="shared" ref="P184:P206" si="34">CONCATENATE("cJSON_AddItemToObject(Uha, ","""",E184,"""",", cJSON_CreateNumber(mVars[",C184,"]));")</f>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS1_CELL1_MV", cJSON_CreateNumber(mVars[180]));</v>
       </c>
     </row>
@@ -5887,26 +6003,26 @@
         <v>190</v>
       </c>
       <c r="H185" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>#define  VAR_BMS1_CELL2_MV  181</v>
       </c>
       <c r="I185" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>public const byte VAR_BMS1_CELL2_MV = 181;</v>
       </c>
       <c r="J185">
         <v>1</v>
       </c>
       <c r="L185" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>UpdateScanList(VAR_BMS1_CELL2_MV, 3000);</v>
       </c>
       <c r="M185" t="str">
-        <f t="shared" ref="M185:M239" si="30">CONCATENATE("VAR_SetVariable(",E185,", Cells[",J185,"].Voltage_mV", ", validflag);")</f>
+        <f t="shared" ref="M185:M239" si="35">CONCATENATE("VAR_SetVariable(",E185,", Cells[",J185,"].Voltage_mV", ", validflag);")</f>
         <v>VAR_SetVariable(VAR_BMS1_CELL2_MV, Cells[1].Voltage_mV, validflag);</v>
       </c>
       <c r="P185" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS1_CELL2_MV", cJSON_CreateNumber(mVars[181]));</v>
       </c>
     </row>
@@ -5922,26 +6038,26 @@
         <v>191</v>
       </c>
       <c r="H186" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>#define  VAR_BMS1_CELL3_MV  182</v>
       </c>
       <c r="I186" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>public const byte VAR_BMS1_CELL3_MV = 182;</v>
       </c>
       <c r="J186">
         <v>2</v>
       </c>
       <c r="L186" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>UpdateScanList(VAR_BMS1_CELL3_MV, 3000);</v>
       </c>
       <c r="M186" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>VAR_SetVariable(VAR_BMS1_CELL3_MV, Cells[2].Voltage_mV, validflag);</v>
       </c>
       <c r="P186" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS1_CELL3_MV", cJSON_CreateNumber(mVars[182]));</v>
       </c>
     </row>
@@ -5957,26 +6073,26 @@
         <v>192</v>
       </c>
       <c r="H187" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>#define  VAR_BMS1_CELL4_MV  183</v>
       </c>
       <c r="I187" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>public const byte VAR_BMS1_CELL4_MV = 183;</v>
       </c>
       <c r="J187">
         <v>3</v>
       </c>
       <c r="L187" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>UpdateScanList(VAR_BMS1_CELL4_MV, 3000);</v>
       </c>
       <c r="M187" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>VAR_SetVariable(VAR_BMS1_CELL4_MV, Cells[3].Voltage_mV, validflag);</v>
       </c>
       <c r="P187" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS1_CELL4_MV", cJSON_CreateNumber(mVars[183]));</v>
       </c>
     </row>
@@ -5992,26 +6108,26 @@
         <v>193</v>
       </c>
       <c r="H188" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>#define  VAR_BMS1_CELL5_MV  184</v>
       </c>
       <c r="I188" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>public const byte VAR_BMS1_CELL5_MV = 184;</v>
       </c>
       <c r="J188">
         <v>4</v>
       </c>
       <c r="L188" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>UpdateScanList(VAR_BMS1_CELL5_MV, 3000);</v>
       </c>
       <c r="M188" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>VAR_SetVariable(VAR_BMS1_CELL5_MV, Cells[4].Voltage_mV, validflag);</v>
       </c>
       <c r="P188" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS1_CELL5_MV", cJSON_CreateNumber(mVars[184]));</v>
       </c>
     </row>
@@ -6027,26 +6143,26 @@
         <v>194</v>
       </c>
       <c r="H189" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>#define  VAR_BMS1_CELL6_MV  185</v>
       </c>
       <c r="I189" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>public const byte VAR_BMS1_CELL6_MV = 185;</v>
       </c>
       <c r="J189">
         <v>5</v>
       </c>
       <c r="L189" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>UpdateScanList(VAR_BMS1_CELL6_MV, 3000);</v>
       </c>
       <c r="M189" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>VAR_SetVariable(VAR_BMS1_CELL6_MV, Cells[5].Voltage_mV, validflag);</v>
       </c>
       <c r="P189" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS1_CELL6_MV", cJSON_CreateNumber(mVars[185]));</v>
       </c>
     </row>
@@ -6062,26 +6178,26 @@
         <v>195</v>
       </c>
       <c r="H190" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>#define  VAR_BMS1_CELL7_MV  186</v>
       </c>
       <c r="I190" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>public const byte VAR_BMS1_CELL7_MV = 186;</v>
       </c>
       <c r="J190">
         <v>6</v>
       </c>
       <c r="L190" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>UpdateScanList(VAR_BMS1_CELL7_MV, 3000);</v>
       </c>
       <c r="M190" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>VAR_SetVariable(VAR_BMS1_CELL7_MV, Cells[6].Voltage_mV, validflag);</v>
       </c>
       <c r="P190" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS1_CELL7_MV", cJSON_CreateNumber(mVars[186]));</v>
       </c>
     </row>
@@ -6097,26 +6213,26 @@
         <v>196</v>
       </c>
       <c r="H191" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>#define  VAR_BMS1_CELL8_MV  187</v>
       </c>
       <c r="I191" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>public const byte VAR_BMS1_CELL8_MV = 187;</v>
       </c>
       <c r="J191">
         <v>7</v>
       </c>
       <c r="L191" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>UpdateScanList(VAR_BMS1_CELL8_MV, 3000);</v>
       </c>
       <c r="M191" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>VAR_SetVariable(VAR_BMS1_CELL8_MV, Cells[7].Voltage_mV, validflag);</v>
       </c>
       <c r="P191" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS1_CELL8_MV", cJSON_CreateNumber(mVars[187]));</v>
       </c>
     </row>
@@ -6132,26 +6248,26 @@
         <v>197</v>
       </c>
       <c r="H192" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>#define  VAR_BMS1_CELL9_MV  188</v>
       </c>
       <c r="I192" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>public const byte VAR_BMS1_CELL9_MV = 188;</v>
       </c>
       <c r="J192">
         <v>8</v>
       </c>
       <c r="L192" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>UpdateScanList(VAR_BMS1_CELL9_MV, 3000);</v>
       </c>
       <c r="M192" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>VAR_SetVariable(VAR_BMS1_CELL9_MV, Cells[8].Voltage_mV, validflag);</v>
       </c>
       <c r="P192" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS1_CELL9_MV", cJSON_CreateNumber(mVars[188]));</v>
       </c>
     </row>
@@ -6167,26 +6283,26 @@
         <v>198</v>
       </c>
       <c r="H193" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>#define  VAR_BMS1_CELL10_MV  189</v>
       </c>
       <c r="I193" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>public const byte VAR_BMS1_CELL10_MV = 189;</v>
       </c>
       <c r="J193">
         <v>9</v>
       </c>
       <c r="L193" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>UpdateScanList(VAR_BMS1_CELL10_MV, 3000);</v>
       </c>
       <c r="M193" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>VAR_SetVariable(VAR_BMS1_CELL10_MV, Cells[9].Voltage_mV, validflag);</v>
       </c>
       <c r="P193" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS1_CELL10_MV", cJSON_CreateNumber(mVars[189]));</v>
       </c>
     </row>
@@ -6202,26 +6318,26 @@
         <v>199</v>
       </c>
       <c r="H194" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>#define  VAR_BMS1_CELL11_MV  190</v>
       </c>
       <c r="I194" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>public const byte VAR_BMS1_CELL11_MV = 190;</v>
       </c>
       <c r="J194">
         <v>10</v>
       </c>
       <c r="L194" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>UpdateScanList(VAR_BMS1_CELL11_MV, 3000);</v>
       </c>
       <c r="M194" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>VAR_SetVariable(VAR_BMS1_CELL11_MV, Cells[10].Voltage_mV, validflag);</v>
       </c>
       <c r="P194" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS1_CELL11_MV", cJSON_CreateNumber(mVars[190]));</v>
       </c>
     </row>
@@ -6237,26 +6353,26 @@
         <v>200</v>
       </c>
       <c r="H195" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>#define  VAR_BMS1_CELL12_MV  191</v>
       </c>
       <c r="I195" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>public const byte VAR_BMS1_CELL12_MV = 191;</v>
       </c>
       <c r="J195">
         <v>11</v>
       </c>
       <c r="L195" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>UpdateScanList(VAR_BMS1_CELL12_MV, 3000);</v>
       </c>
       <c r="M195" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>VAR_SetVariable(VAR_BMS1_CELL12_MV, Cells[11].Voltage_mV, validflag);</v>
       </c>
       <c r="P195" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS1_CELL12_MV", cJSON_CreateNumber(mVars[191]));</v>
       </c>
     </row>
@@ -6272,26 +6388,26 @@
         <v>201</v>
       </c>
       <c r="H196" t="str">
-        <f t="shared" ref="H196:H255" si="31">CONCATENATE("#define  ",E196,"  ",C196)</f>
+        <f t="shared" ref="H196:H255" si="36">CONCATENATE("#define  ",E196,"  ",C196)</f>
         <v>#define  VAR_BMS1_CELL13_MV  192</v>
       </c>
       <c r="I196" t="str">
-        <f t="shared" ref="I196:I255" si="32">CONCATENATE("public const byte ",E196," = ",C196,";")</f>
+        <f t="shared" ref="I196:I255" si="37">CONCATENATE("public const byte ",E196," = ",C196,";")</f>
         <v>public const byte VAR_BMS1_CELL13_MV = 192;</v>
       </c>
       <c r="J196">
         <v>12</v>
       </c>
       <c r="L196" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>UpdateScanList(VAR_BMS1_CELL13_MV, 3000);</v>
       </c>
       <c r="M196" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>VAR_SetVariable(VAR_BMS1_CELL13_MV, Cells[12].Voltage_mV, validflag);</v>
       </c>
       <c r="P196" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS1_CELL13_MV", cJSON_CreateNumber(mVars[192]));</v>
       </c>
     </row>
@@ -6300,33 +6416,33 @@
         <v>193</v>
       </c>
       <c r="D197" s="1" t="str">
-        <f t="shared" ref="D197:D259" si="33">DEC2HEX(C197,2)</f>
+        <f t="shared" ref="D197:D259" si="38">DEC2HEX(C197,2)</f>
         <v>C1</v>
       </c>
       <c r="E197" t="s">
         <v>202</v>
       </c>
       <c r="H197" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS1_CELL14_MV  193</v>
       </c>
       <c r="I197" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS1_CELL14_MV = 193;</v>
       </c>
       <c r="J197">
         <v>13</v>
       </c>
       <c r="L197" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>UpdateScanList(VAR_BMS1_CELL14_MV, 3000);</v>
       </c>
       <c r="M197" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>VAR_SetVariable(VAR_BMS1_CELL14_MV, Cells[13].Voltage_mV, validflag);</v>
       </c>
       <c r="P197" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS1_CELL14_MV", cJSON_CreateNumber(mVars[193]));</v>
       </c>
     </row>
@@ -6335,33 +6451,33 @@
         <v>194</v>
       </c>
       <c r="D198" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>C2</v>
       </c>
       <c r="E198" t="s">
         <v>203</v>
       </c>
       <c r="H198" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS1_CELL15_MV  194</v>
       </c>
       <c r="I198" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS1_CELL15_MV = 194;</v>
       </c>
       <c r="J198">
         <v>14</v>
       </c>
       <c r="L198" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>UpdateScanList(VAR_BMS1_CELL15_MV, 3000);</v>
       </c>
       <c r="M198" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>VAR_SetVariable(VAR_BMS1_CELL15_MV, Cells[14].Voltage_mV, validflag);</v>
       </c>
       <c r="P198" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS1_CELL15_MV", cJSON_CreateNumber(mVars[194]));</v>
       </c>
     </row>
@@ -6370,33 +6486,33 @@
         <v>195</v>
       </c>
       <c r="D199" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>C3</v>
       </c>
       <c r="E199" t="s">
         <v>204</v>
       </c>
       <c r="H199" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS1_CELL16_MV  195</v>
       </c>
       <c r="I199" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS1_CELL16_MV = 195;</v>
       </c>
       <c r="J199">
         <v>15</v>
       </c>
       <c r="L199" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>UpdateScanList(VAR_BMS1_CELL16_MV, 3000);</v>
       </c>
       <c r="M199" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>VAR_SetVariable(VAR_BMS1_CELL16_MV, Cells[15].Voltage_mV, validflag);</v>
       </c>
       <c r="P199" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS1_CELL16_MV", cJSON_CreateNumber(mVars[195]));</v>
       </c>
     </row>
@@ -6405,25 +6521,25 @@
         <v>196</v>
       </c>
       <c r="D200" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>C4</v>
       </c>
       <c r="E200" t="s">
         <v>221</v>
       </c>
       <c r="H200" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS1_CELL1_C  196</v>
       </c>
       <c r="I200" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS1_CELL1_C = 196;</v>
       </c>
       <c r="J200">
         <v>0</v>
       </c>
       <c r="L200" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>UpdateScanList(VAR_BMS1_CELL1_C, 3000);</v>
       </c>
       <c r="M200" t="str">
@@ -6431,7 +6547,7 @@
         <v>VAR_SetVariable(VAR_BMS1_CELL1_C, Cells[0].Temp_C, validflag);</v>
       </c>
       <c r="P200" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS1_CELL1_C", cJSON_CreateNumber(mVars[196]));</v>
       </c>
     </row>
@@ -6440,33 +6556,33 @@
         <v>197</v>
       </c>
       <c r="D201" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>C5</v>
       </c>
       <c r="E201" t="s">
         <v>222</v>
       </c>
       <c r="H201" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS1_CELL2_C  197</v>
       </c>
       <c r="I201" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS1_CELL2_C = 197;</v>
       </c>
       <c r="J201">
         <v>1</v>
       </c>
       <c r="L201" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>UpdateScanList(VAR_BMS1_CELL2_C, 3000);</v>
       </c>
       <c r="M201" t="str">
-        <f t="shared" ref="M201:M215" si="34">CONCATENATE("VAR_SetVariable(",E201,", Cells[",J201,"].Temp_C", ", validflag);")</f>
+        <f t="shared" ref="M201:M215" si="39">CONCATENATE("VAR_SetVariable(",E201,", Cells[",J201,"].Temp_C", ", validflag);")</f>
         <v>VAR_SetVariable(VAR_BMS1_CELL2_C, Cells[1].Temp_C, validflag);</v>
       </c>
       <c r="P201" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS1_CELL2_C", cJSON_CreateNumber(mVars[197]));</v>
       </c>
     </row>
@@ -6475,33 +6591,33 @@
         <v>198</v>
       </c>
       <c r="D202" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>C6</v>
       </c>
       <c r="E202" t="s">
         <v>223</v>
       </c>
       <c r="H202" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS1_CELL3_C  198</v>
       </c>
       <c r="I202" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS1_CELL3_C = 198;</v>
       </c>
       <c r="J202">
         <v>2</v>
       </c>
       <c r="L202" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>UpdateScanList(VAR_BMS1_CELL3_C, 3000);</v>
       </c>
       <c r="M202" t="str">
+        <f t="shared" si="39"/>
+        <v>VAR_SetVariable(VAR_BMS1_CELL3_C, Cells[2].Temp_C, validflag);</v>
+      </c>
+      <c r="P202" t="str">
         <f t="shared" si="34"/>
-        <v>VAR_SetVariable(VAR_BMS1_CELL3_C, Cells[2].Temp_C, validflag);</v>
-      </c>
-      <c r="P202" t="str">
-        <f t="shared" si="29"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS1_CELL3_C", cJSON_CreateNumber(mVars[198]));</v>
       </c>
     </row>
@@ -6510,33 +6626,33 @@
         <v>199</v>
       </c>
       <c r="D203" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>C7</v>
       </c>
       <c r="E203" t="s">
         <v>224</v>
       </c>
       <c r="H203" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS1_CELL4_C  199</v>
       </c>
       <c r="I203" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS1_CELL4_C = 199;</v>
       </c>
       <c r="J203">
         <v>3</v>
       </c>
       <c r="L203" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>UpdateScanList(VAR_BMS1_CELL4_C, 3000);</v>
       </c>
       <c r="M203" t="str">
+        <f t="shared" si="39"/>
+        <v>VAR_SetVariable(VAR_BMS1_CELL4_C, Cells[3].Temp_C, validflag);</v>
+      </c>
+      <c r="P203" t="str">
         <f t="shared" si="34"/>
-        <v>VAR_SetVariable(VAR_BMS1_CELL4_C, Cells[3].Temp_C, validflag);</v>
-      </c>
-      <c r="P203" t="str">
-        <f t="shared" si="29"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS1_CELL4_C", cJSON_CreateNumber(mVars[199]));</v>
       </c>
     </row>
@@ -6545,33 +6661,33 @@
         <v>200</v>
       </c>
       <c r="D204" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>C8</v>
       </c>
       <c r="E204" t="s">
         <v>225</v>
       </c>
       <c r="H204" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS1_CELL5_C  200</v>
       </c>
       <c r="I204" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS1_CELL5_C = 200;</v>
       </c>
       <c r="J204">
         <v>4</v>
       </c>
       <c r="L204" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>UpdateScanList(VAR_BMS1_CELL5_C, 3000);</v>
       </c>
       <c r="M204" t="str">
+        <f t="shared" si="39"/>
+        <v>VAR_SetVariable(VAR_BMS1_CELL5_C, Cells[4].Temp_C, validflag);</v>
+      </c>
+      <c r="P204" t="str">
         <f t="shared" si="34"/>
-        <v>VAR_SetVariable(VAR_BMS1_CELL5_C, Cells[4].Temp_C, validflag);</v>
-      </c>
-      <c r="P204" t="str">
-        <f t="shared" si="29"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS1_CELL5_C", cJSON_CreateNumber(mVars[200]));</v>
       </c>
     </row>
@@ -6580,33 +6696,33 @@
         <v>201</v>
       </c>
       <c r="D205" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>C9</v>
       </c>
       <c r="E205" t="s">
         <v>226</v>
       </c>
       <c r="H205" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS1_CELL6_C  201</v>
       </c>
       <c r="I205" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS1_CELL6_C = 201;</v>
       </c>
       <c r="J205">
         <v>5</v>
       </c>
       <c r="L205" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>UpdateScanList(VAR_BMS1_CELL6_C, 3000);</v>
       </c>
       <c r="M205" t="str">
+        <f t="shared" si="39"/>
+        <v>VAR_SetVariable(VAR_BMS1_CELL6_C, Cells[5].Temp_C, validflag);</v>
+      </c>
+      <c r="P205" t="str">
         <f t="shared" si="34"/>
-        <v>VAR_SetVariable(VAR_BMS1_CELL6_C, Cells[5].Temp_C, validflag);</v>
-      </c>
-      <c r="P205" t="str">
-        <f t="shared" si="29"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS1_CELL6_C", cJSON_CreateNumber(mVars[201]));</v>
       </c>
     </row>
@@ -6615,33 +6731,33 @@
         <v>202</v>
       </c>
       <c r="D206" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>CA</v>
       </c>
       <c r="E206" t="s">
         <v>227</v>
       </c>
       <c r="H206" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS1_CELL7_C  202</v>
       </c>
       <c r="I206" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS1_CELL7_C = 202;</v>
       </c>
       <c r="J206">
         <v>6</v>
       </c>
       <c r="L206" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>UpdateScanList(VAR_BMS1_CELL7_C, 3000);</v>
       </c>
       <c r="M206" t="str">
+        <f t="shared" si="39"/>
+        <v>VAR_SetVariable(VAR_BMS1_CELL7_C, Cells[6].Temp_C, validflag);</v>
+      </c>
+      <c r="P206" t="str">
         <f t="shared" si="34"/>
-        <v>VAR_SetVariable(VAR_BMS1_CELL7_C, Cells[6].Temp_C, validflag);</v>
-      </c>
-      <c r="P206" t="str">
-        <f t="shared" si="29"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS1_CELL7_C", cJSON_CreateNumber(mVars[202]));</v>
       </c>
     </row>
@@ -6650,33 +6766,33 @@
         <v>203</v>
       </c>
       <c r="D207" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>CB</v>
       </c>
       <c r="E207" t="s">
         <v>228</v>
       </c>
       <c r="H207" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS1_CELL8_C  203</v>
       </c>
       <c r="I207" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS1_CELL8_C = 203;</v>
       </c>
       <c r="J207">
         <v>7</v>
       </c>
       <c r="L207" t="str">
-        <f t="shared" ref="L207:L255" si="35">CONCATENATE("UpdateScanList(",E207, ", 3000);")</f>
+        <f t="shared" ref="L207:L255" si="40">CONCATENATE("UpdateScanList(",E207, ", 3000);")</f>
         <v>UpdateScanList(VAR_BMS1_CELL8_C, 3000);</v>
       </c>
       <c r="M207" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>VAR_SetVariable(VAR_BMS1_CELL8_C, Cells[7].Temp_C, validflag);</v>
       </c>
       <c r="P207" t="str">
-        <f t="shared" ref="P207:P255" si="36">CONCATENATE("cJSON_AddItemToObject(Uha, ","""",E207,"""",", cJSON_CreateNumber(mVars[",C207,"]));")</f>
+        <f t="shared" ref="P207:P255" si="41">CONCATENATE("cJSON_AddItemToObject(Uha, ","""",E207,"""",", cJSON_CreateNumber(mVars[",C207,"]));")</f>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS1_CELL8_C", cJSON_CreateNumber(mVars[203]));</v>
       </c>
     </row>
@@ -6685,33 +6801,33 @@
         <v>204</v>
       </c>
       <c r="D208" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>CC</v>
       </c>
       <c r="E208" t="s">
         <v>229</v>
       </c>
       <c r="H208" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS1_CELL9_C  204</v>
       </c>
       <c r="I208" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS1_CELL9_C = 204;</v>
       </c>
       <c r="J208">
         <v>8</v>
       </c>
       <c r="L208" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>UpdateScanList(VAR_BMS1_CELL9_C, 3000);</v>
       </c>
       <c r="M208" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>VAR_SetVariable(VAR_BMS1_CELL9_C, Cells[8].Temp_C, validflag);</v>
       </c>
       <c r="P208" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS1_CELL9_C", cJSON_CreateNumber(mVars[204]));</v>
       </c>
     </row>
@@ -6720,33 +6836,33 @@
         <v>205</v>
       </c>
       <c r="D209" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>CD</v>
       </c>
       <c r="E209" t="s">
         <v>230</v>
       </c>
       <c r="H209" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS1_CELL10_C  205</v>
       </c>
       <c r="I209" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS1_CELL10_C = 205;</v>
       </c>
       <c r="J209">
         <v>9</v>
       </c>
       <c r="L209" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>UpdateScanList(VAR_BMS1_CELL10_C, 3000);</v>
       </c>
       <c r="M209" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>VAR_SetVariable(VAR_BMS1_CELL10_C, Cells[9].Temp_C, validflag);</v>
       </c>
       <c r="P209" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS1_CELL10_C", cJSON_CreateNumber(mVars[205]));</v>
       </c>
     </row>
@@ -6755,33 +6871,33 @@
         <v>206</v>
       </c>
       <c r="D210" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>CE</v>
       </c>
       <c r="E210" t="s">
         <v>231</v>
       </c>
       <c r="H210" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS1_CELL11_C  206</v>
       </c>
       <c r="I210" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS1_CELL11_C = 206;</v>
       </c>
       <c r="J210">
         <v>10</v>
       </c>
       <c r="L210" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>UpdateScanList(VAR_BMS1_CELL11_C, 3000);</v>
       </c>
       <c r="M210" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>VAR_SetVariable(VAR_BMS1_CELL11_C, Cells[10].Temp_C, validflag);</v>
       </c>
       <c r="P210" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS1_CELL11_C", cJSON_CreateNumber(mVars[206]));</v>
       </c>
     </row>
@@ -6790,33 +6906,33 @@
         <v>207</v>
       </c>
       <c r="D211" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>CF</v>
       </c>
       <c r="E211" t="s">
         <v>232</v>
       </c>
       <c r="H211" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS1_CELL12_C  207</v>
       </c>
       <c r="I211" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS1_CELL12_C = 207;</v>
       </c>
       <c r="J211">
         <v>11</v>
       </c>
       <c r="L211" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>UpdateScanList(VAR_BMS1_CELL12_C, 3000);</v>
       </c>
       <c r="M211" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>VAR_SetVariable(VAR_BMS1_CELL12_C, Cells[11].Temp_C, validflag);</v>
       </c>
       <c r="P211" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS1_CELL12_C", cJSON_CreateNumber(mVars[207]));</v>
       </c>
     </row>
@@ -6825,33 +6941,33 @@
         <v>208</v>
       </c>
       <c r="D212" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>D0</v>
       </c>
       <c r="E212" t="s">
         <v>233</v>
       </c>
       <c r="H212" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS1_CELL13_C  208</v>
       </c>
       <c r="I212" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS1_CELL13_C = 208;</v>
       </c>
       <c r="J212">
         <v>12</v>
       </c>
       <c r="L212" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>UpdateScanList(VAR_BMS1_CELL13_C, 3000);</v>
       </c>
       <c r="M212" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>VAR_SetVariable(VAR_BMS1_CELL13_C, Cells[12].Temp_C, validflag);</v>
       </c>
       <c r="P212" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS1_CELL13_C", cJSON_CreateNumber(mVars[208]));</v>
       </c>
     </row>
@@ -6860,33 +6976,33 @@
         <v>209</v>
       </c>
       <c r="D213" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>D1</v>
       </c>
       <c r="E213" t="s">
         <v>234</v>
       </c>
       <c r="H213" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS1_CELL14_C  209</v>
       </c>
       <c r="I213" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS1_CELL14_C = 209;</v>
       </c>
       <c r="J213">
         <v>13</v>
       </c>
       <c r="L213" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>UpdateScanList(VAR_BMS1_CELL14_C, 3000);</v>
       </c>
       <c r="M213" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>VAR_SetVariable(VAR_BMS1_CELL14_C, Cells[13].Temp_C, validflag);</v>
       </c>
       <c r="P213" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS1_CELL14_C", cJSON_CreateNumber(mVars[209]));</v>
       </c>
     </row>
@@ -6895,33 +7011,33 @@
         <v>210</v>
       </c>
       <c r="D214" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>D2</v>
       </c>
       <c r="E214" t="s">
         <v>235</v>
       </c>
       <c r="H214" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS1_CELL15_C  210</v>
       </c>
       <c r="I214" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS1_CELL15_C = 210;</v>
       </c>
       <c r="J214">
         <v>14</v>
       </c>
       <c r="L214" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>UpdateScanList(VAR_BMS1_CELL15_C, 3000);</v>
       </c>
       <c r="M214" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>VAR_SetVariable(VAR_BMS1_CELL15_C, Cells[14].Temp_C, validflag);</v>
       </c>
       <c r="P214" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS1_CELL15_C", cJSON_CreateNumber(mVars[210]));</v>
       </c>
     </row>
@@ -6930,33 +7046,33 @@
         <v>211</v>
       </c>
       <c r="D215" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>D3</v>
       </c>
       <c r="E215" t="s">
         <v>236</v>
       </c>
       <c r="H215" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS1_CELL16_C  211</v>
       </c>
       <c r="I215" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS1_CELL16_C = 211;</v>
       </c>
       <c r="J215">
         <v>15</v>
       </c>
       <c r="L215" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>UpdateScanList(VAR_BMS1_CELL16_C, 3000);</v>
       </c>
       <c r="M215" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>VAR_SetVariable(VAR_BMS1_CELL16_C, Cells[15].Temp_C, validflag);</v>
       </c>
       <c r="P215" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS1_CELL16_C", cJSON_CreateNumber(mVars[211]));</v>
       </c>
     </row>
@@ -6965,7 +7081,7 @@
         <v>212</v>
       </c>
       <c r="D216" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>D4</v>
       </c>
     </row>
@@ -6974,7 +7090,7 @@
         <v>213</v>
       </c>
       <c r="D217" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>D5</v>
       </c>
     </row>
@@ -6983,7 +7099,7 @@
         <v>214</v>
       </c>
       <c r="D218" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>D6</v>
       </c>
     </row>
@@ -6992,7 +7108,7 @@
         <v>215</v>
       </c>
       <c r="D219" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>D7</v>
       </c>
     </row>
@@ -7001,7 +7117,7 @@
         <v>216</v>
       </c>
       <c r="D220" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>D8</v>
       </c>
     </row>
@@ -7010,7 +7126,7 @@
         <v>217</v>
       </c>
       <c r="D221" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>D9</v>
       </c>
     </row>
@@ -7019,7 +7135,7 @@
         <v>218</v>
       </c>
       <c r="D222" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>DA</v>
       </c>
     </row>
@@ -7028,7 +7144,7 @@
         <v>219</v>
       </c>
       <c r="D223" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>DB</v>
       </c>
     </row>
@@ -7037,33 +7153,33 @@
         <v>220</v>
       </c>
       <c r="D224" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>DC</v>
       </c>
       <c r="E224" t="s">
         <v>205</v>
       </c>
       <c r="H224" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS2_CELL1_MV  220</v>
       </c>
       <c r="I224" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS2_CELL1_MV = 220;</v>
       </c>
       <c r="J224">
         <v>0</v>
       </c>
       <c r="L224" t="str">
+        <f t="shared" si="40"/>
+        <v>UpdateScanList(VAR_BMS2_CELL1_MV, 3000);</v>
+      </c>
+      <c r="M224" t="str">
         <f t="shared" si="35"/>
-        <v>UpdateScanList(VAR_BMS2_CELL1_MV, 3000);</v>
-      </c>
-      <c r="M224" t="str">
-        <f t="shared" si="30"/>
         <v>VAR_SetVariable(VAR_BMS2_CELL1_MV, Cells[0].Voltage_mV, validflag);</v>
       </c>
       <c r="P224" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS2_CELL1_MV", cJSON_CreateNumber(mVars[220]));</v>
       </c>
     </row>
@@ -7072,33 +7188,33 @@
         <v>221</v>
       </c>
       <c r="D225" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>DD</v>
       </c>
       <c r="E225" t="s">
         <v>206</v>
       </c>
       <c r="H225" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS2_CELL2_MV  221</v>
       </c>
       <c r="I225" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS2_CELL2_MV = 221;</v>
       </c>
       <c r="J225">
         <v>1</v>
       </c>
       <c r="L225" t="str">
+        <f t="shared" si="40"/>
+        <v>UpdateScanList(VAR_BMS2_CELL2_MV, 3000);</v>
+      </c>
+      <c r="M225" t="str">
         <f t="shared" si="35"/>
-        <v>UpdateScanList(VAR_BMS2_CELL2_MV, 3000);</v>
-      </c>
-      <c r="M225" t="str">
-        <f t="shared" si="30"/>
         <v>VAR_SetVariable(VAR_BMS2_CELL2_MV, Cells[1].Voltage_mV, validflag);</v>
       </c>
       <c r="P225" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS2_CELL2_MV", cJSON_CreateNumber(mVars[221]));</v>
       </c>
     </row>
@@ -7107,33 +7223,33 @@
         <v>222</v>
       </c>
       <c r="D226" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>DE</v>
       </c>
       <c r="E226" t="s">
         <v>207</v>
       </c>
       <c r="H226" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS2_CELL3_MV  222</v>
       </c>
       <c r="I226" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS2_CELL3_MV = 222;</v>
       </c>
       <c r="J226">
         <v>2</v>
       </c>
       <c r="L226" t="str">
+        <f t="shared" si="40"/>
+        <v>UpdateScanList(VAR_BMS2_CELL3_MV, 3000);</v>
+      </c>
+      <c r="M226" t="str">
         <f t="shared" si="35"/>
-        <v>UpdateScanList(VAR_BMS2_CELL3_MV, 3000);</v>
-      </c>
-      <c r="M226" t="str">
-        <f t="shared" si="30"/>
         <v>VAR_SetVariable(VAR_BMS2_CELL3_MV, Cells[2].Voltage_mV, validflag);</v>
       </c>
       <c r="P226" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS2_CELL3_MV", cJSON_CreateNumber(mVars[222]));</v>
       </c>
     </row>
@@ -7142,33 +7258,33 @@
         <v>223</v>
       </c>
       <c r="D227" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>DF</v>
       </c>
       <c r="E227" t="s">
         <v>208</v>
       </c>
       <c r="H227" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS2_CELL4_MV  223</v>
       </c>
       <c r="I227" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS2_CELL4_MV = 223;</v>
       </c>
       <c r="J227">
         <v>3</v>
       </c>
       <c r="L227" t="str">
+        <f t="shared" si="40"/>
+        <v>UpdateScanList(VAR_BMS2_CELL4_MV, 3000);</v>
+      </c>
+      <c r="M227" t="str">
         <f t="shared" si="35"/>
-        <v>UpdateScanList(VAR_BMS2_CELL4_MV, 3000);</v>
-      </c>
-      <c r="M227" t="str">
-        <f t="shared" si="30"/>
         <v>VAR_SetVariable(VAR_BMS2_CELL4_MV, Cells[3].Voltage_mV, validflag);</v>
       </c>
       <c r="P227" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS2_CELL4_MV", cJSON_CreateNumber(mVars[223]));</v>
       </c>
     </row>
@@ -7177,33 +7293,33 @@
         <v>224</v>
       </c>
       <c r="D228" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>E0</v>
       </c>
       <c r="E228" t="s">
         <v>209</v>
       </c>
       <c r="H228" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS2_CELL5_MV  224</v>
       </c>
       <c r="I228" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS2_CELL5_MV = 224;</v>
       </c>
       <c r="J228">
         <v>4</v>
       </c>
       <c r="L228" t="str">
+        <f t="shared" si="40"/>
+        <v>UpdateScanList(VAR_BMS2_CELL5_MV, 3000);</v>
+      </c>
+      <c r="M228" t="str">
         <f t="shared" si="35"/>
-        <v>UpdateScanList(VAR_BMS2_CELL5_MV, 3000);</v>
-      </c>
-      <c r="M228" t="str">
-        <f t="shared" si="30"/>
         <v>VAR_SetVariable(VAR_BMS2_CELL5_MV, Cells[4].Voltage_mV, validflag);</v>
       </c>
       <c r="P228" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS2_CELL5_MV", cJSON_CreateNumber(mVars[224]));</v>
       </c>
     </row>
@@ -7212,33 +7328,33 @@
         <v>225</v>
       </c>
       <c r="D229" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>E1</v>
       </c>
       <c r="E229" t="s">
         <v>210</v>
       </c>
       <c r="H229" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS2_CELL6_MV  225</v>
       </c>
       <c r="I229" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS2_CELL6_MV = 225;</v>
       </c>
       <c r="J229">
         <v>5</v>
       </c>
       <c r="L229" t="str">
+        <f t="shared" si="40"/>
+        <v>UpdateScanList(VAR_BMS2_CELL6_MV, 3000);</v>
+      </c>
+      <c r="M229" t="str">
         <f t="shared" si="35"/>
-        <v>UpdateScanList(VAR_BMS2_CELL6_MV, 3000);</v>
-      </c>
-      <c r="M229" t="str">
-        <f t="shared" si="30"/>
         <v>VAR_SetVariable(VAR_BMS2_CELL6_MV, Cells[5].Voltage_mV, validflag);</v>
       </c>
       <c r="P229" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS2_CELL6_MV", cJSON_CreateNumber(mVars[225]));</v>
       </c>
     </row>
@@ -7247,33 +7363,33 @@
         <v>226</v>
       </c>
       <c r="D230" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>E2</v>
       </c>
       <c r="E230" t="s">
         <v>211</v>
       </c>
       <c r="H230" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS2_CELL7_MV  226</v>
       </c>
       <c r="I230" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS2_CELL7_MV = 226;</v>
       </c>
       <c r="J230">
         <v>6</v>
       </c>
       <c r="L230" t="str">
+        <f t="shared" si="40"/>
+        <v>UpdateScanList(VAR_BMS2_CELL7_MV, 3000);</v>
+      </c>
+      <c r="M230" t="str">
         <f t="shared" si="35"/>
-        <v>UpdateScanList(VAR_BMS2_CELL7_MV, 3000);</v>
-      </c>
-      <c r="M230" t="str">
-        <f t="shared" si="30"/>
         <v>VAR_SetVariable(VAR_BMS2_CELL7_MV, Cells[6].Voltage_mV, validflag);</v>
       </c>
       <c r="P230" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS2_CELL7_MV", cJSON_CreateNumber(mVars[226]));</v>
       </c>
     </row>
@@ -7282,33 +7398,33 @@
         <v>227</v>
       </c>
       <c r="D231" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>E3</v>
       </c>
       <c r="E231" t="s">
         <v>212</v>
       </c>
       <c r="H231" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS2_CELL8_MV  227</v>
       </c>
       <c r="I231" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS2_CELL8_MV = 227;</v>
       </c>
       <c r="J231">
         <v>7</v>
       </c>
       <c r="L231" t="str">
+        <f t="shared" si="40"/>
+        <v>UpdateScanList(VAR_BMS2_CELL8_MV, 3000);</v>
+      </c>
+      <c r="M231" t="str">
         <f t="shared" si="35"/>
-        <v>UpdateScanList(VAR_BMS2_CELL8_MV, 3000);</v>
-      </c>
-      <c r="M231" t="str">
-        <f t="shared" si="30"/>
         <v>VAR_SetVariable(VAR_BMS2_CELL8_MV, Cells[7].Voltage_mV, validflag);</v>
       </c>
       <c r="P231" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS2_CELL8_MV", cJSON_CreateNumber(mVars[227]));</v>
       </c>
     </row>
@@ -7317,33 +7433,33 @@
         <v>228</v>
       </c>
       <c r="D232" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>E4</v>
       </c>
       <c r="E232" t="s">
         <v>213</v>
       </c>
       <c r="H232" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS2_CELL9_MV  228</v>
       </c>
       <c r="I232" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS2_CELL9_MV = 228;</v>
       </c>
       <c r="J232">
         <v>8</v>
       </c>
       <c r="L232" t="str">
+        <f t="shared" si="40"/>
+        <v>UpdateScanList(VAR_BMS2_CELL9_MV, 3000);</v>
+      </c>
+      <c r="M232" t="str">
         <f t="shared" si="35"/>
-        <v>UpdateScanList(VAR_BMS2_CELL9_MV, 3000);</v>
-      </c>
-      <c r="M232" t="str">
-        <f t="shared" si="30"/>
         <v>VAR_SetVariable(VAR_BMS2_CELL9_MV, Cells[8].Voltage_mV, validflag);</v>
       </c>
       <c r="P232" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS2_CELL9_MV", cJSON_CreateNumber(mVars[228]));</v>
       </c>
     </row>
@@ -7352,33 +7468,33 @@
         <v>229</v>
       </c>
       <c r="D233" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>E5</v>
       </c>
       <c r="E233" t="s">
         <v>214</v>
       </c>
       <c r="H233" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS2_CELL10_MV  229</v>
       </c>
       <c r="I233" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS2_CELL10_MV = 229;</v>
       </c>
       <c r="J233">
         <v>9</v>
       </c>
       <c r="L233" t="str">
+        <f t="shared" si="40"/>
+        <v>UpdateScanList(VAR_BMS2_CELL10_MV, 3000);</v>
+      </c>
+      <c r="M233" t="str">
         <f t="shared" si="35"/>
-        <v>UpdateScanList(VAR_BMS2_CELL10_MV, 3000);</v>
-      </c>
-      <c r="M233" t="str">
-        <f t="shared" si="30"/>
         <v>VAR_SetVariable(VAR_BMS2_CELL10_MV, Cells[9].Voltage_mV, validflag);</v>
       </c>
       <c r="P233" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS2_CELL10_MV", cJSON_CreateNumber(mVars[229]));</v>
       </c>
     </row>
@@ -7387,33 +7503,33 @@
         <v>230</v>
       </c>
       <c r="D234" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>E6</v>
       </c>
       <c r="E234" t="s">
         <v>215</v>
       </c>
       <c r="H234" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS2_CELL11_MV  230</v>
       </c>
       <c r="I234" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS2_CELL11_MV = 230;</v>
       </c>
       <c r="J234">
         <v>10</v>
       </c>
       <c r="L234" t="str">
+        <f t="shared" si="40"/>
+        <v>UpdateScanList(VAR_BMS2_CELL11_MV, 3000);</v>
+      </c>
+      <c r="M234" t="str">
         <f t="shared" si="35"/>
-        <v>UpdateScanList(VAR_BMS2_CELL11_MV, 3000);</v>
-      </c>
-      <c r="M234" t="str">
-        <f t="shared" si="30"/>
         <v>VAR_SetVariable(VAR_BMS2_CELL11_MV, Cells[10].Voltage_mV, validflag);</v>
       </c>
       <c r="P234" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS2_CELL11_MV", cJSON_CreateNumber(mVars[230]));</v>
       </c>
     </row>
@@ -7422,33 +7538,33 @@
         <v>231</v>
       </c>
       <c r="D235" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>E7</v>
       </c>
       <c r="E235" t="s">
         <v>216</v>
       </c>
       <c r="H235" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS2_CELL12_MV  231</v>
       </c>
       <c r="I235" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS2_CELL12_MV = 231;</v>
       </c>
       <c r="J235">
         <v>11</v>
       </c>
       <c r="L235" t="str">
+        <f t="shared" si="40"/>
+        <v>UpdateScanList(VAR_BMS2_CELL12_MV, 3000);</v>
+      </c>
+      <c r="M235" t="str">
         <f t="shared" si="35"/>
-        <v>UpdateScanList(VAR_BMS2_CELL12_MV, 3000);</v>
-      </c>
-      <c r="M235" t="str">
-        <f t="shared" si="30"/>
         <v>VAR_SetVariable(VAR_BMS2_CELL12_MV, Cells[11].Voltage_mV, validflag);</v>
       </c>
       <c r="P235" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS2_CELL12_MV", cJSON_CreateNumber(mVars[231]));</v>
       </c>
     </row>
@@ -7457,33 +7573,33 @@
         <v>232</v>
       </c>
       <c r="D236" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>E8</v>
       </c>
       <c r="E236" t="s">
         <v>217</v>
       </c>
       <c r="H236" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS2_CELL13_MV  232</v>
       </c>
       <c r="I236" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS2_CELL13_MV = 232;</v>
       </c>
       <c r="J236">
         <v>12</v>
       </c>
       <c r="L236" t="str">
+        <f t="shared" si="40"/>
+        <v>UpdateScanList(VAR_BMS2_CELL13_MV, 3000);</v>
+      </c>
+      <c r="M236" t="str">
         <f t="shared" si="35"/>
-        <v>UpdateScanList(VAR_BMS2_CELL13_MV, 3000);</v>
-      </c>
-      <c r="M236" t="str">
-        <f t="shared" si="30"/>
         <v>VAR_SetVariable(VAR_BMS2_CELL13_MV, Cells[12].Voltage_mV, validflag);</v>
       </c>
       <c r="P236" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS2_CELL13_MV", cJSON_CreateNumber(mVars[232]));</v>
       </c>
     </row>
@@ -7492,33 +7608,33 @@
         <v>233</v>
       </c>
       <c r="D237" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>E9</v>
       </c>
       <c r="E237" t="s">
         <v>218</v>
       </c>
       <c r="H237" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS2_CELL14_MV  233</v>
       </c>
       <c r="I237" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS2_CELL14_MV = 233;</v>
       </c>
       <c r="J237">
         <v>13</v>
       </c>
       <c r="L237" t="str">
+        <f t="shared" si="40"/>
+        <v>UpdateScanList(VAR_BMS2_CELL14_MV, 3000);</v>
+      </c>
+      <c r="M237" t="str">
         <f t="shared" si="35"/>
-        <v>UpdateScanList(VAR_BMS2_CELL14_MV, 3000);</v>
-      </c>
-      <c r="M237" t="str">
-        <f t="shared" si="30"/>
         <v>VAR_SetVariable(VAR_BMS2_CELL14_MV, Cells[13].Voltage_mV, validflag);</v>
       </c>
       <c r="P237" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS2_CELL14_MV", cJSON_CreateNumber(mVars[233]));</v>
       </c>
     </row>
@@ -7527,33 +7643,33 @@
         <v>234</v>
       </c>
       <c r="D238" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>EA</v>
       </c>
       <c r="E238" t="s">
         <v>219</v>
       </c>
       <c r="H238" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS2_CELL15_MV  234</v>
       </c>
       <c r="I238" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS2_CELL15_MV = 234;</v>
       </c>
       <c r="J238">
         <v>14</v>
       </c>
       <c r="L238" t="str">
+        <f t="shared" si="40"/>
+        <v>UpdateScanList(VAR_BMS2_CELL15_MV, 3000);</v>
+      </c>
+      <c r="M238" t="str">
         <f t="shared" si="35"/>
-        <v>UpdateScanList(VAR_BMS2_CELL15_MV, 3000);</v>
-      </c>
-      <c r="M238" t="str">
-        <f t="shared" si="30"/>
         <v>VAR_SetVariable(VAR_BMS2_CELL15_MV, Cells[14].Voltage_mV, validflag);</v>
       </c>
       <c r="P238" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS2_CELL15_MV", cJSON_CreateNumber(mVars[234]));</v>
       </c>
     </row>
@@ -7562,33 +7678,33 @@
         <v>235</v>
       </c>
       <c r="D239" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>EB</v>
       </c>
       <c r="E239" t="s">
         <v>220</v>
       </c>
       <c r="H239" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS2_CELL16_MV  235</v>
       </c>
       <c r="I239" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS2_CELL16_MV = 235;</v>
       </c>
       <c r="J239">
         <v>15</v>
       </c>
       <c r="L239" t="str">
+        <f t="shared" si="40"/>
+        <v>UpdateScanList(VAR_BMS2_CELL16_MV, 3000);</v>
+      </c>
+      <c r="M239" t="str">
         <f t="shared" si="35"/>
-        <v>UpdateScanList(VAR_BMS2_CELL16_MV, 3000);</v>
-      </c>
-      <c r="M239" t="str">
-        <f t="shared" si="30"/>
         <v>VAR_SetVariable(VAR_BMS2_CELL16_MV, Cells[15].Voltage_mV, validflag);</v>
       </c>
       <c r="P239" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS2_CELL16_MV", cJSON_CreateNumber(mVars[235]));</v>
       </c>
     </row>
@@ -7597,25 +7713,25 @@
         <v>236</v>
       </c>
       <c r="D240" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>EC</v>
       </c>
       <c r="E240" t="s">
         <v>237</v>
       </c>
       <c r="H240" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS2_CELL1_C  236</v>
       </c>
       <c r="I240" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS2_CELL1_C = 236;</v>
       </c>
       <c r="J240">
         <v>0</v>
       </c>
       <c r="L240" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>UpdateScanList(VAR_BMS2_CELL1_C, 3000);</v>
       </c>
       <c r="M240" t="str">
@@ -7623,7 +7739,7 @@
         <v>VAR_SetVariable(VAR_BMS2_CELL1_C, Cells[0].Temp_C, validflag);</v>
       </c>
       <c r="P240" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS2_CELL1_C", cJSON_CreateNumber(mVars[236]));</v>
       </c>
     </row>
@@ -7632,33 +7748,33 @@
         <v>237</v>
       </c>
       <c r="D241" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>ED</v>
       </c>
       <c r="E241" t="s">
         <v>238</v>
       </c>
       <c r="H241" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS2_CELL2_C  237</v>
       </c>
       <c r="I241" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS2_CELL2_C = 237;</v>
       </c>
       <c r="J241">
         <v>1</v>
       </c>
       <c r="L241" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>UpdateScanList(VAR_BMS2_CELL2_C, 3000);</v>
       </c>
       <c r="M241" t="str">
-        <f t="shared" ref="M241:M255" si="37">CONCATENATE("VAR_SetVariable(",E241,", Cells[",J241,"].Temp_C", ", validflag);")</f>
+        <f t="shared" ref="M241:M255" si="42">CONCATENATE("VAR_SetVariable(",E241,", Cells[",J241,"].Temp_C", ", validflag);")</f>
         <v>VAR_SetVariable(VAR_BMS2_CELL2_C, Cells[1].Temp_C, validflag);</v>
       </c>
       <c r="P241" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS2_CELL2_C", cJSON_CreateNumber(mVars[237]));</v>
       </c>
     </row>
@@ -7667,33 +7783,33 @@
         <v>238</v>
       </c>
       <c r="D242" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>EE</v>
       </c>
       <c r="E242" t="s">
         <v>239</v>
       </c>
       <c r="H242" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS2_CELL3_C  238</v>
       </c>
       <c r="I242" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS2_CELL3_C = 238;</v>
       </c>
       <c r="J242">
         <v>2</v>
       </c>
       <c r="L242" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>UpdateScanList(VAR_BMS2_CELL3_C, 3000);</v>
       </c>
       <c r="M242" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="42"/>
         <v>VAR_SetVariable(VAR_BMS2_CELL3_C, Cells[2].Temp_C, validflag);</v>
       </c>
       <c r="P242" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS2_CELL3_C", cJSON_CreateNumber(mVars[238]));</v>
       </c>
     </row>
@@ -7702,33 +7818,33 @@
         <v>239</v>
       </c>
       <c r="D243" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>EF</v>
       </c>
       <c r="E243" t="s">
         <v>240</v>
       </c>
       <c r="H243" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS2_CELL4_C  239</v>
       </c>
       <c r="I243" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS2_CELL4_C = 239;</v>
       </c>
       <c r="J243">
         <v>3</v>
       </c>
       <c r="L243" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>UpdateScanList(VAR_BMS2_CELL4_C, 3000);</v>
       </c>
       <c r="M243" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="42"/>
         <v>VAR_SetVariable(VAR_BMS2_CELL4_C, Cells[3].Temp_C, validflag);</v>
       </c>
       <c r="P243" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS2_CELL4_C", cJSON_CreateNumber(mVars[239]));</v>
       </c>
     </row>
@@ -7737,33 +7853,33 @@
         <v>240</v>
       </c>
       <c r="D244" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>F0</v>
       </c>
       <c r="E244" t="s">
         <v>241</v>
       </c>
       <c r="H244" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS2_CELL5_C  240</v>
       </c>
       <c r="I244" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS2_CELL5_C = 240;</v>
       </c>
       <c r="J244">
         <v>4</v>
       </c>
       <c r="L244" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>UpdateScanList(VAR_BMS2_CELL5_C, 3000);</v>
       </c>
       <c r="M244" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="42"/>
         <v>VAR_SetVariable(VAR_BMS2_CELL5_C, Cells[4].Temp_C, validflag);</v>
       </c>
       <c r="P244" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS2_CELL5_C", cJSON_CreateNumber(mVars[240]));</v>
       </c>
     </row>
@@ -7772,33 +7888,33 @@
         <v>241</v>
       </c>
       <c r="D245" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>F1</v>
       </c>
       <c r="E245" t="s">
         <v>242</v>
       </c>
       <c r="H245" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS2_CELL6_C  241</v>
       </c>
       <c r="I245" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS2_CELL6_C = 241;</v>
       </c>
       <c r="J245">
         <v>5</v>
       </c>
       <c r="L245" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>UpdateScanList(VAR_BMS2_CELL6_C, 3000);</v>
       </c>
       <c r="M245" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="42"/>
         <v>VAR_SetVariable(VAR_BMS2_CELL6_C, Cells[5].Temp_C, validflag);</v>
       </c>
       <c r="P245" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS2_CELL6_C", cJSON_CreateNumber(mVars[241]));</v>
       </c>
     </row>
@@ -7807,33 +7923,33 @@
         <v>242</v>
       </c>
       <c r="D246" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>F2</v>
       </c>
       <c r="E246" t="s">
         <v>243</v>
       </c>
       <c r="H246" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS2_CELL7_C  242</v>
       </c>
       <c r="I246" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS2_CELL7_C = 242;</v>
       </c>
       <c r="J246">
         <v>6</v>
       </c>
       <c r="L246" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>UpdateScanList(VAR_BMS2_CELL7_C, 3000);</v>
       </c>
       <c r="M246" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="42"/>
         <v>VAR_SetVariable(VAR_BMS2_CELL7_C, Cells[6].Temp_C, validflag);</v>
       </c>
       <c r="P246" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS2_CELL7_C", cJSON_CreateNumber(mVars[242]));</v>
       </c>
     </row>
@@ -7842,33 +7958,33 @@
         <v>243</v>
       </c>
       <c r="D247" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>F3</v>
       </c>
       <c r="E247" t="s">
         <v>244</v>
       </c>
       <c r="H247" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS2_CELL8_C  243</v>
       </c>
       <c r="I247" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS2_CELL8_C = 243;</v>
       </c>
       <c r="J247">
         <v>7</v>
       </c>
       <c r="L247" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>UpdateScanList(VAR_BMS2_CELL8_C, 3000);</v>
       </c>
       <c r="M247" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="42"/>
         <v>VAR_SetVariable(VAR_BMS2_CELL8_C, Cells[7].Temp_C, validflag);</v>
       </c>
       <c r="P247" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS2_CELL8_C", cJSON_CreateNumber(mVars[243]));</v>
       </c>
     </row>
@@ -7877,33 +7993,33 @@
         <v>244</v>
       </c>
       <c r="D248" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>F4</v>
       </c>
       <c r="E248" t="s">
         <v>245</v>
       </c>
       <c r="H248" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS2_CELL9_C  244</v>
       </c>
       <c r="I248" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS2_CELL9_C = 244;</v>
       </c>
       <c r="J248">
         <v>8</v>
       </c>
       <c r="L248" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>UpdateScanList(VAR_BMS2_CELL9_C, 3000);</v>
       </c>
       <c r="M248" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="42"/>
         <v>VAR_SetVariable(VAR_BMS2_CELL9_C, Cells[8].Temp_C, validflag);</v>
       </c>
       <c r="P248" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS2_CELL9_C", cJSON_CreateNumber(mVars[244]));</v>
       </c>
     </row>
@@ -7912,33 +8028,33 @@
         <v>245</v>
       </c>
       <c r="D249" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>F5</v>
       </c>
       <c r="E249" t="s">
         <v>246</v>
       </c>
       <c r="H249" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS2_CELL10_C  245</v>
       </c>
       <c r="I249" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS2_CELL10_C = 245;</v>
       </c>
       <c r="J249">
         <v>9</v>
       </c>
       <c r="L249" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>UpdateScanList(VAR_BMS2_CELL10_C, 3000);</v>
       </c>
       <c r="M249" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="42"/>
         <v>VAR_SetVariable(VAR_BMS2_CELL10_C, Cells[9].Temp_C, validflag);</v>
       </c>
       <c r="P249" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS2_CELL10_C", cJSON_CreateNumber(mVars[245]));</v>
       </c>
     </row>
@@ -7947,33 +8063,33 @@
         <v>246</v>
       </c>
       <c r="D250" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>F6</v>
       </c>
       <c r="E250" t="s">
         <v>247</v>
       </c>
       <c r="H250" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS2_CELL11_C  246</v>
       </c>
       <c r="I250" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS2_CELL11_C = 246;</v>
       </c>
       <c r="J250">
         <v>10</v>
       </c>
       <c r="L250" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>UpdateScanList(VAR_BMS2_CELL11_C, 3000);</v>
       </c>
       <c r="M250" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="42"/>
         <v>VAR_SetVariable(VAR_BMS2_CELL11_C, Cells[10].Temp_C, validflag);</v>
       </c>
       <c r="P250" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS2_CELL11_C", cJSON_CreateNumber(mVars[246]));</v>
       </c>
     </row>
@@ -7982,33 +8098,33 @@
         <v>247</v>
       </c>
       <c r="D251" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>F7</v>
       </c>
       <c r="E251" t="s">
         <v>248</v>
       </c>
       <c r="H251" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS2_CELL12_C  247</v>
       </c>
       <c r="I251" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS2_CELL12_C = 247;</v>
       </c>
       <c r="J251">
         <v>11</v>
       </c>
       <c r="L251" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>UpdateScanList(VAR_BMS2_CELL12_C, 3000);</v>
       </c>
       <c r="M251" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="42"/>
         <v>VAR_SetVariable(VAR_BMS2_CELL12_C, Cells[11].Temp_C, validflag);</v>
       </c>
       <c r="P251" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS2_CELL12_C", cJSON_CreateNumber(mVars[247]));</v>
       </c>
     </row>
@@ -8017,33 +8133,33 @@
         <v>248</v>
       </c>
       <c r="D252" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>F8</v>
       </c>
       <c r="E252" t="s">
         <v>249</v>
       </c>
       <c r="H252" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS2_CELL13_C  248</v>
       </c>
       <c r="I252" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS2_CELL13_C = 248;</v>
       </c>
       <c r="J252">
         <v>12</v>
       </c>
       <c r="L252" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>UpdateScanList(VAR_BMS2_CELL13_C, 3000);</v>
       </c>
       <c r="M252" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="42"/>
         <v>VAR_SetVariable(VAR_BMS2_CELL13_C, Cells[12].Temp_C, validflag);</v>
       </c>
       <c r="P252" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS2_CELL13_C", cJSON_CreateNumber(mVars[248]));</v>
       </c>
     </row>
@@ -8052,33 +8168,33 @@
         <v>249</v>
       </c>
       <c r="D253" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>F9</v>
       </c>
       <c r="E253" t="s">
         <v>250</v>
       </c>
       <c r="H253" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS2_CELL14_C  249</v>
       </c>
       <c r="I253" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS2_CELL14_C = 249;</v>
       </c>
       <c r="J253">
         <v>13</v>
       </c>
       <c r="L253" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>UpdateScanList(VAR_BMS2_CELL14_C, 3000);</v>
       </c>
       <c r="M253" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="42"/>
         <v>VAR_SetVariable(VAR_BMS2_CELL14_C, Cells[13].Temp_C, validflag);</v>
       </c>
       <c r="P253" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS2_CELL14_C", cJSON_CreateNumber(mVars[249]));</v>
       </c>
     </row>
@@ -8087,33 +8203,33 @@
         <v>250</v>
       </c>
       <c r="D254" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>FA</v>
       </c>
       <c r="E254" t="s">
         <v>251</v>
       </c>
       <c r="H254" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS2_CELL15_C  250</v>
       </c>
       <c r="I254" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS2_CELL15_C = 250;</v>
       </c>
       <c r="J254">
         <v>14</v>
       </c>
       <c r="L254" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>UpdateScanList(VAR_BMS2_CELL15_C, 3000);</v>
       </c>
       <c r="M254" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="42"/>
         <v>VAR_SetVariable(VAR_BMS2_CELL15_C, Cells[14].Temp_C, validflag);</v>
       </c>
       <c r="P254" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS2_CELL15_C", cJSON_CreateNumber(mVars[250]));</v>
       </c>
     </row>
@@ -8122,33 +8238,33 @@
         <v>251</v>
       </c>
       <c r="D255" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>FB</v>
       </c>
       <c r="E255" t="s">
         <v>252</v>
       </c>
       <c r="H255" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>#define  VAR_BMS2_CELL16_C  251</v>
       </c>
       <c r="I255" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>public const byte VAR_BMS2_CELL16_C = 251;</v>
       </c>
       <c r="J255">
         <v>15</v>
       </c>
       <c r="L255" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>UpdateScanList(VAR_BMS2_CELL16_C, 3000);</v>
       </c>
       <c r="M255" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="42"/>
         <v>VAR_SetVariable(VAR_BMS2_CELL16_C, Cells[15].Temp_C, validflag);</v>
       </c>
       <c r="P255" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>cJSON_AddItemToObject(Uha, "VAR_BMS2_CELL16_C", cJSON_CreateNumber(mVars[251]));</v>
       </c>
     </row>
@@ -8157,7 +8273,7 @@
         <v>252</v>
       </c>
       <c r="D256" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>FC</v>
       </c>
     </row>
@@ -8166,7 +8282,7 @@
         <v>253</v>
       </c>
       <c r="D257" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>FD</v>
       </c>
     </row>
@@ -8175,7 +8291,7 @@
         <v>254</v>
       </c>
       <c r="D258" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>FE</v>
       </c>
     </row>
@@ -8184,7 +8300,7 @@
         <v>255</v>
       </c>
       <c r="D259" s="1" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>FF</v>
       </c>
     </row>

</xml_diff>